<commit_message>
Finalizada la sección 4 del curso
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -96,13 +96,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,6 +156,1289 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>158750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F9892B7-2EDA-4091-B976-2B9CC1320EAF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>215900</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDB4A3FB-2AC2-4EB0-B88B-762507858744}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0646E1B-139E-47C3-9A56-A27B7D0736BB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>158750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07EF3E80-1842-4FA3-98DB-5777A62CCD52}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>215900</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E701BAE-8C88-41AE-B528-4BC079415357}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08390486-6F45-4E99-AC03-D116C0DEF92B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDC48C01-5955-46E9-AA03-0387E71617FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>215900</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E6279D-A70A-4392-A078-D96AE3C263F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>31750</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3C9336-1425-46CD-A52E-A79E5CD28D55}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9E0B2D-8065-4586-8FBD-375F4DAEDC59}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF786F75-E50F-4088-A3AC-6A36476B9BFC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>44450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49E128E4-8C32-45D3-A4DC-7B42120A43D9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C1F817-D17F-4348-8728-7A7D70771910}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>165100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD304F53-2422-490F-9527-8BDF23AD90F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>215900</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC310EC-D4F9-4483-8DEA-139B144340DD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>222250</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>425450</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F53244D-ABE0-4587-ACC6-0B402F951450}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>165100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76831D80-4526-4536-AA2E-69EC3E4E95E0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>431800</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>165100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE1EB9B-8C91-413C-92BD-D9C1CD7429D6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,11 +1737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,6 +1775,7 @@
       <c r="C2" s="2">
         <v>43255</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -498,6 +1787,7 @@
       <c r="C3" s="2">
         <v>43263</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -509,6 +1799,7 @@
       <c r="C4" s="2">
         <v>43269</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -520,6 +1811,7 @@
       <c r="C5" s="2">
         <v>43277</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -527,6 +1819,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -534,6 +1827,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -541,6 +1835,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -548,6 +1843,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -555,6 +1851,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -562,6 +1859,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -569,6 +1867,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -576,6 +1875,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -583,6 +1883,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -590,6 +1891,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -597,30 +1899,438 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>158750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId6" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId7" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>158750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId8" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId9" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId10" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId11" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId12" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>31750</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>6350</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId13" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId14" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId15" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>44450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1037" r:id="rId16" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1038" r:id="rId17" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>6350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>165100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1039" r:id="rId18" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1040" r:id="rId19" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>177800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1041" r:id="rId20" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>6350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>165100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" r:id="rId21" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>6350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>165100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>